<commit_message>
Creating first version bot
Signed-off-by: jamarcolan <zn_john@hotmail.com>
</commit_message>
<xml_diff>
--- a/Novo(a) Planilha do Microsoft Excel.xlsx
+++ b/Novo(a) Planilha do Microsoft Excel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52534F9C-0AD8-4CFF-9BBA-942D9027AE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6527DEB-A39A-4EAA-9A2B-D02AC6612B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6105" yWindow="1320" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5355" yWindow="2460" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>sell_qnt_eur</t>
   </si>
@@ -58,6 +59,21 @@
   </si>
   <si>
     <t>profit</t>
+  </si>
+  <si>
+    <t>Buy_price</t>
+  </si>
+  <si>
+    <t>Sell_price</t>
+  </si>
+  <si>
+    <t>qnt_dolar</t>
+  </si>
+  <si>
+    <t>Buy euro</t>
+  </si>
+  <si>
+    <t>Sell euro</t>
   </si>
 </sst>
 </file>
@@ -393,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,4 +607,66 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30470002-3BBF-4E64-8F7B-5C0B8EE57B97}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.1040000000000001</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <f>B2*A2</f>
+        <v>11.040000000000001</v>
+      </c>
+      <c r="D2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E2">
+        <f>C2/D2</f>
+        <v>9.9459459459459456</v>
+      </c>
+      <c r="F2">
+        <f>E2*D2</f>
+        <v>11.040000000000001</v>
+      </c>
+      <c r="G2">
+        <f>B2-E2</f>
+        <v>5.405405405405439E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add airflow and dags.
Signed-off-by: jamarcolan <zn_john@hotmail.com>
</commit_message>
<xml_diff>
--- a/Novo(a) Planilha do Microsoft Excel.xlsx
+++ b/Novo(a) Planilha do Microsoft Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bots\binance_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6527DEB-A39A-4EAA-9A2B-D02AC6612B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8087BE9-A240-47E7-928A-8BEC87429E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="2460" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -611,10 +611,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30470002-3BBF-4E64-8F7B-5C0B8EE57B97}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,6 +666,33 @@
         <v>5.405405405405439E-2</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.05</v>
+      </c>
+      <c r="B3">
+        <v>11.9</v>
+      </c>
+      <c r="C3">
+        <f>B3*A3</f>
+        <v>12.495000000000001</v>
+      </c>
+      <c r="D3">
+        <v>1.054</v>
+      </c>
+      <c r="E3">
+        <f>C3/D3</f>
+        <v>11.85483870967742</v>
+      </c>
+      <c r="F3">
+        <f>E3*D3</f>
+        <v>12.495000000000001</v>
+      </c>
+      <c r="G3">
+        <f>B3-E3</f>
+        <v>4.5161290322580427E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>